<commit_message>
adding bln $ detail
</commit_message>
<xml_diff>
--- a/ship_industry_revenue_gross_output.xlsx
+++ b/ship_industry_revenue_gross_output.xlsx
@@ -1,17 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivynyayieka/Downloads/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5365612-1C3C-B742-9EEB-EE0DD1AA094F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="labour_by_year" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Sheet2" sheetId="3" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="labour_by_year" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$A$1:$Z$14</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">labour_by_year!$A$1:$AA$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">labour_by_year!$A$1:$AA$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Z$14</definedName>
   </definedNames>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -72,44 +82,50 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="&quot;Source Sans Pro Web&quot;"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF4F4F4F"/>
       <name val="-apple-system"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF4F4F4F"/>
       <name val="-apple-system"/>
     </font>
@@ -119,7 +135,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -135,72 +151,86 @@
     </fill>
   </fills>
   <borders count="3">
-    <border/>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FFAAAAAA"/>
       </right>
+      <top/>
       <bottom style="thick">
         <color rgb="FFD9D9D9"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="3" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+  <cellXfs count="11">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="2" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="1"/>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -217,7 +247,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0">
+              <a:rPr lang="en-US" b="0">
                 <a:solidFill>
                   <a:srgbClr val="757575"/>
                 </a:solidFill>
@@ -230,9 +260,11 @@
       </c:tx>
       <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -240,6 +272,12 @@
           <c:tx>
             <c:strRef>
               <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ship building and repairing</c:v>
+                </c:pt>
+              </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -255,16 +293,114 @@
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$A$2:$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2018*</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2019*</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2020*</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2021*</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2022*</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2023*</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2024*</c:v>
+                </c:pt>
+              </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$B$2:$B$14</c:f>
-              <c:numCache/>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>24.95</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25.68</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24.79</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24.81</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>23.61</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24.84</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24.97</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22.33</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>22.98</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>25.39</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>25.47</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-94FB-7043-B999-B2A3941C8418}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
         <c:axId val="430937400"/>
         <c:axId val="918795000"/>
       </c:lineChart>
@@ -290,7 +426,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0">
+                  <a:rPr lang="en-US" b="0">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -306,7 +442,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:spPr/>
+        <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
           <a:lstStyle/>
@@ -319,9 +455,15 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="918795000"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="918795000"/>
@@ -365,7 +507,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0">
+                  <a:rPr lang="en-US" b="0">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -397,9 +539,12 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="430937400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -417,16 +562,28 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="1"/>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -443,7 +600,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0">
+              <a:rPr lang="en-US" b="0">
                 <a:solidFill>
                   <a:srgbClr val="757575"/>
                 </a:solidFill>
@@ -456,9 +613,11 @@
       </c:tx>
       <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -474,18 +633,63 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>labour_by_year!$B$9:$B$12</c:f>
-            </c:strRef>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2022</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:f>labour_by_year!$E$9:$E$12</c:f>
-              <c:numCache/>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>140770</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>137110</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>144540</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>147950</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E117-3847-83A3-59153EDBEDA3}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
         <c:axId val="574748632"/>
         <c:axId val="1147373450"/>
       </c:lineChart>
@@ -510,15 +714,7 @@
                     <a:latin typeface="+mn-lt"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:r>
-                  <a:rPr b="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:rPr>
-                  <a:t/>
-                </a:r>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -527,7 +723,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:spPr/>
+        <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
           <a:lstStyle/>
@@ -540,9 +736,15 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1147373450"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="1147373450"/>
@@ -574,21 +776,13 @@
                     <a:latin typeface="+mn-lt"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:r>
-                  <a:rPr b="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:rPr>
-                  <a:t/>
-                </a:r>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -609,9 +803,12 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="574748632"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -629,16 +826,28 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="1"/>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -655,22 +864,39 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0">
+              <a:rPr lang="en-US" b="0">
                 <a:solidFill>
                   <a:srgbClr val="757575"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
               </a:rPr>
-              <a:t>Gross output from shipbuilding and repair has trended up since 2016</a:t>
+              <a:t>Gross output from shipbuilding and repair has trended up since 2016 (in</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" b="0" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:rPr>
+              <a:t> billion USD)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" b="0">
+              <a:solidFill>
+                <a:srgbClr val="757575"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
       <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -678,6 +904,12 @@
           <c:tx>
             <c:strRef>
               <c:f>Sheet2!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Gross Output</c:v>
+                </c:pt>
+              </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -691,18 +923,87 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>Sheet2!$B$1:$I$1</c:f>
-            </c:strRef>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2021</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet2!$B$2:$I$2</c:f>
-              <c:numCache/>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>23.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24.7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>26.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>31.2</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9ABC-C44F-8476-C15D64D58695}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
         <c:axId val="704394741"/>
         <c:axId val="787867981"/>
       </c:lineChart>
@@ -728,7 +1029,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0">
+                  <a:rPr lang="en-US" b="0">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -744,7 +1045,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:spPr/>
+        <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
           <a:lstStyle/>
@@ -757,9 +1058,15 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="787867981"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="787867981"/>
@@ -803,7 +1110,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0">
+                  <a:rPr lang="en-US" b="0">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -835,9 +1142,12 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="704394741"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -855,16 +1165,24 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
@@ -873,9 +1191,15 @@
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5715000" cy="3533775"/>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="1" name="Chart 1" title="Chart"/>
+        <xdr:cNvPr id="2" name="Chart 1" title="Chart">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -884,7 +1208,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -894,7 +1218,7 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
@@ -903,9 +1227,15 @@
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5715000" cy="3533775"/>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 2" title="Chart"/>
+        <xdr:cNvPr id="2" name="Chart 2" title="Chart">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -914,7 +1244,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -924,7 +1254,7 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
@@ -933,9 +1263,15 @@
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5715000" cy="3533775"/>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 3" title="Chart"/>
+        <xdr:cNvPr id="3" name="Chart 3" title="Chart">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -944,7 +1280,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -954,7 +1290,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1144,20 +1480,25 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1168,9 +1509,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" ht="15.75" customHeight="1">
       <c r="A2" s="4">
-        <v>2012.0</v>
+        <v>2012</v>
       </c>
       <c r="B2" s="3">
         <v>24.95</v>
@@ -1179,9 +1520,9 @@
         <v>7.13</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:3" ht="15.75" customHeight="1">
       <c r="A3" s="4">
-        <v>2013.0</v>
+        <v>2013</v>
       </c>
       <c r="B3" s="3">
         <v>25.68</v>
@@ -1190,9 +1531,9 @@
         <v>7.89</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:3" ht="15.75" customHeight="1">
       <c r="A4" s="4">
-        <v>2014.0</v>
+        <v>2014</v>
       </c>
       <c r="B4" s="3">
         <v>24.79</v>
@@ -1201,9 +1542,9 @@
         <v>8.61</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:3" ht="15.75" customHeight="1">
       <c r="A5" s="4">
-        <v>2015.0</v>
+        <v>2015</v>
       </c>
       <c r="B5" s="3">
         <v>24.81</v>
@@ -1212,9 +1553,9 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:3" ht="15.75" customHeight="1">
       <c r="A6" s="4">
-        <v>2016.0</v>
+        <v>2016</v>
       </c>
       <c r="B6" s="3">
         <v>23.61</v>
@@ -1223,9 +1564,9 @@
         <v>9.76</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:3" ht="15.75" customHeight="1">
       <c r="A7" s="4">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="B7" s="3">
         <v>24.7</v>
@@ -1234,7 +1575,7 @@
         <v>10.26</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:3" ht="15.75" customHeight="1">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
@@ -1245,7 +1586,7 @@
         <v>10.57</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:3" ht="15.75" customHeight="1">
       <c r="A9" s="4" t="s">
         <v>4</v>
       </c>
@@ -1256,7 +1597,7 @@
         <v>10.86</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:3" ht="15.75" customHeight="1">
       <c r="A10" s="4" t="s">
         <v>5</v>
       </c>
@@ -1267,7 +1608,7 @@
         <v>9.9</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:3" ht="15.75" customHeight="1">
       <c r="A11" s="4" t="s">
         <v>6</v>
       </c>
@@ -1278,18 +1619,18 @@
         <v>10.36</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:3" ht="15.75" customHeight="1">
       <c r="A12" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="3">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="C12" s="3">
         <v>10.98</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:3" ht="15.75" customHeight="1">
       <c r="A13" s="4" t="s">
         <v>8</v>
       </c>
@@ -1300,7 +1641,7 @@
         <v>11.77</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:3" ht="15.75" customHeight="1">
       <c r="A14" s="4" t="s">
         <v>9</v>
       </c>
@@ -1312,27 +1653,24 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="$A$1:$Z$14">
-    <sortState ref="A1:Z14">
-      <sortCondition ref="A1:A14"/>
-      <sortCondition descending="1" ref="B1:B14"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:Z14" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1349,12 +1687,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="4">
-        <v>2012.0</v>
+        <v>2012</v>
       </c>
       <c r="B2" s="4">
-        <v>2012.0</v>
+        <v>2012</v>
       </c>
       <c r="C2" s="3">
         <v>24.95</v>
@@ -1363,12 +1701,12 @@
         <v>7.13</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="A3" s="4">
-        <v>2013.0</v>
+        <v>2013</v>
       </c>
       <c r="B3" s="4">
-        <v>2013.0</v>
+        <v>2013</v>
       </c>
       <c r="C3" s="3">
         <v>25.68</v>
@@ -1377,12 +1715,12 @@
         <v>7.89</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="A4" s="4">
-        <v>2014.0</v>
+        <v>2014</v>
       </c>
       <c r="B4" s="4">
-        <v>2014.0</v>
+        <v>2014</v>
       </c>
       <c r="C4" s="3">
         <v>24.79</v>
@@ -1391,12 +1729,12 @@
         <v>8.61</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1">
       <c r="A5" s="4">
-        <v>2015.0</v>
+        <v>2015</v>
       </c>
       <c r="B5" s="4">
-        <v>2015.0</v>
+        <v>2015</v>
       </c>
       <c r="C5" s="3">
         <v>24.81</v>
@@ -1405,12 +1743,12 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1">
       <c r="A6" s="4">
-        <v>2016.0</v>
+        <v>2016</v>
       </c>
       <c r="B6" s="4">
-        <v>2016.0</v>
+        <v>2016</v>
       </c>
       <c r="C6" s="3">
         <v>23.61</v>
@@ -1419,12 +1757,12 @@
         <v>9.76</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1">
       <c r="A7" s="4">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="B7" s="4">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="C7" s="3">
         <v>24.7</v>
@@ -1433,12 +1771,12 @@
         <v>10.26</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="4">
-        <v>2018.0</v>
+        <v>2018</v>
       </c>
       <c r="C8" s="3">
         <v>24.84</v>
@@ -1447,12 +1785,12 @@
         <v>10.57</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1">
       <c r="A9" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="4">
-        <v>2019.0</v>
+        <v>2019</v>
       </c>
       <c r="C9" s="3">
         <v>24.97</v>
@@ -1461,18 +1799,18 @@
         <v>10.86</v>
       </c>
       <c r="E9" s="6">
-        <v>140770.0</v>
+        <v>140770</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:6" ht="15.75" customHeight="1">
       <c r="A10" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="4">
-        <v>2020.0</v>
+        <v>2020</v>
       </c>
       <c r="C10" s="3">
         <v>22.33</v>
@@ -1481,18 +1819,18 @@
         <v>9.9</v>
       </c>
       <c r="E10" s="6">
-        <v>137110.0</v>
+        <v>137110</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:6" ht="15.75" customHeight="1">
       <c r="A11" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="4">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="C11" s="3">
         <v>22.98</v>
@@ -1501,35 +1839,35 @@
         <v>10.36</v>
       </c>
       <c r="E11" s="6">
-        <v>144540.0</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>144540</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" customHeight="1">
       <c r="A12" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="4">
-        <v>2022.0</v>
+        <v>2022</v>
       </c>
       <c r="C12" s="3">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="D12" s="3">
         <v>10.98</v>
       </c>
-      <c r="E12" s="8">
-        <v>147950.0</v>
+      <c r="E12" s="6">
+        <v>147950</v>
       </c>
       <c r="F12" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:6" ht="15.75" customHeight="1">
       <c r="A13" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="4">
-        <v>2023.0</v>
+        <v>2023</v>
       </c>
       <c r="C13" s="3">
         <v>25.39</v>
@@ -1537,14 +1875,14 @@
       <c r="D13" s="3">
         <v>11.77</v>
       </c>
-      <c r="E13" s="9"/>
-    </row>
-    <row r="14">
+      <c r="E13" s="8"/>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" customHeight="1">
       <c r="A14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="4">
-        <v>2024.0</v>
+        <v>2024</v>
       </c>
       <c r="C14" s="3">
         <v>25.47</v>
@@ -1554,90 +1892,90 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="$A$1:$AA$14">
-    <sortState ref="A1:AA14">
-      <sortCondition ref="A1:A14"/>
-      <sortCondition descending="1" ref="C1:C14"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:AA14" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="F9"/>
-    <hyperlink r:id="rId2" ref="F10"/>
-    <hyperlink r:id="rId3" ref="F12"/>
+    <hyperlink ref="F9" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="F10" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="F12" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
   </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:9">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10">
-        <v>2014.0</v>
-      </c>
-      <c r="C1" s="10">
-        <v>2015.0</v>
-      </c>
-      <c r="D1" s="10">
-        <v>2016.0</v>
-      </c>
-      <c r="E1" s="10">
-        <v>2017.0</v>
-      </c>
-      <c r="F1" s="10">
-        <v>2018.0</v>
-      </c>
-      <c r="G1" s="10">
-        <v>2019.0</v>
-      </c>
-      <c r="H1" s="10">
-        <v>2020.0</v>
-      </c>
-      <c r="I1" s="10">
-        <v>2021.0</v>
-      </c>
-    </row>
-    <row r="2">
+      <c r="B1" s="9">
+        <v>2014</v>
+      </c>
+      <c r="C1" s="9">
+        <v>2015</v>
+      </c>
+      <c r="D1" s="9">
+        <v>2016</v>
+      </c>
+      <c r="E1" s="9">
+        <v>2017</v>
+      </c>
+      <c r="F1" s="9">
+        <v>2018</v>
+      </c>
+      <c r="G1" s="9">
+        <v>2019</v>
+      </c>
+      <c r="H1" s="9">
+        <v>2020</v>
+      </c>
+      <c r="I1" s="9">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="11">
+      <c r="B2" s="10">
         <v>23.8</v>
       </c>
-      <c r="C2" s="11">
+      <c r="C2" s="10">
         <v>26.1</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="10">
         <v>24.5</v>
       </c>
-      <c r="E2" s="11">
+      <c r="E2" s="10">
         <v>24.8</v>
       </c>
-      <c r="F2" s="11">
+      <c r="F2" s="10">
         <v>24.7</v>
       </c>
-      <c r="G2" s="11">
+      <c r="G2" s="10">
         <v>26.7</v>
       </c>
-      <c r="H2" s="11">
+      <c r="H2" s="10">
         <v>27.4</v>
       </c>
-      <c r="I2" s="11">
+      <c r="I2" s="10">
         <v>31.2</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
with darker excel pics + dark notification
</commit_message>
<xml_diff>
--- a/ship_industry_revenue_gross_output.xlsx
+++ b/ship_industry_revenue_gross_output.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivynyayieka/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivynyayieka/Downloads/ship_3d-main/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28F47963-32E9-F54D-B96D-7D9C36C5B04F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3917C229-2E8A-644D-8CF2-BED948188F2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -587,35 +587,81 @@
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="1"/>
-  <c:style val="2"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
         <c:rich>
-          <a:bodyPr/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
-            <a:pPr lvl="0">
-              <a:defRPr b="0">
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
                 <a:solidFill>
-                  <a:srgbClr val="757575"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
                 </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
                 <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" b="0">
-                <a:solidFill>
-                  <a:srgbClr val="757575"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-              </a:rPr>
+              <a:rPr lang="en-US"/>
               <a:t>Slight annual increase in total employment in ship and boat building since 2020</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
       <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -627,15 +673,79 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln cmpd="sng">
+            <a:ln w="34925" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="4285F4"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
+              <a:round/>
             </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="95000"/>
+                          <a:alpha val="54000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:numRef>
               <c:f>labour_by_year!$B$9:$B$12</c:f>
@@ -686,8 +796,9 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="ctr"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -707,15 +818,19 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr/>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
-                <a:pPr lvl="0">
-                  <a:defRPr b="0">
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
-                      <a:srgbClr val="000000"/>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:endParaRPr lang="en-US"/>
@@ -723,21 +838,64 @@
             </c:rich>
           </c:tx>
           <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="10000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
         <c:txPr>
-          <a:bodyPr/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
-            <a:pPr lvl="0">
-              <a:defRPr b="0">
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:srgbClr val="000000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -754,30 +912,40 @@
         <c:axId val="1147373450"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:ln>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:srgbClr val="B7B7B7"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
               </a:solidFill>
+              <a:round/>
             </a:ln>
+            <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr/>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
-                <a:pPr lvl="0">
-                  <a:defRPr b="0">
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
-                      <a:srgbClr val="000000"/>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:endParaRPr lang="en-US"/>
@@ -785,26 +953,58 @@
             </c:rich>
           </c:tx>
           <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
+          <a:noFill/>
           <a:ln>
-            <a:solidFill/>
+            <a:noFill/>
           </a:ln>
+          <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
-            <a:pPr lvl="0">
-              <a:defRPr b="0">
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:srgbClr val="000000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -814,30 +1014,54 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0">
-            <a:defRPr b="0">
-              <a:solidFill>
-                <a:srgbClr val="1A1A1A"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
     <c:showDLblsOverMax val="1"/>
   </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -851,50 +1075,81 @@
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="1"/>
-  <c:style val="2"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
         <c:rich>
-          <a:bodyPr/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
-            <a:pPr lvl="0">
-              <a:defRPr b="0">
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
                 <a:solidFill>
-                  <a:srgbClr val="757575"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
                 </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
                 <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" b="0">
-                <a:solidFill>
-                  <a:srgbClr val="757575"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-              </a:rPr>
-              <a:t>Gross output from shipbuilding and repair has trended up since 2016 (in</a:t>
+              <a:rPr lang="en-US"/>
+              <a:t>Gross output from shipbuilding and repair has trended up since 2016 (in billion USD)</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" b="0" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="757575"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-              </a:rPr>
-              <a:t> billion USD)</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US" b="0">
-              <a:solidFill>
-                <a:srgbClr val="757575"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
       <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -917,15 +1172,79 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln cmpd="sng">
+            <a:ln w="34925" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="4285F4"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
+              <a:round/>
             </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="95000"/>
+                          <a:alpha val="54000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:numRef>
               <c:f>Sheet2!$B$1:$I$1</c:f>
@@ -1000,8 +1319,9 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="ctr"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -1021,45 +1341,87 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr/>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
-                <a:pPr lvl="0">
-                  <a:defRPr b="0">
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
-                      <a:srgbClr val="000000"/>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" b="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:rPr>
+                  <a:rPr lang="en-US"/>
                   <a:t>Year</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
           <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="10000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
         <c:txPr>
-          <a:bodyPr/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
-            <a:pPr lvl="0">
-              <a:defRPr b="0">
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:srgbClr val="000000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -1081,69 +1443,96 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:ln>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:srgbClr val="B7B7B7"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
               </a:solidFill>
+              <a:round/>
             </a:ln>
+            <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:minorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="CCCCCC">
-                  <a:alpha val="0"/>
-                </a:srgbClr>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:minorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr/>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
-                <a:pPr lvl="0">
-                  <a:defRPr b="0">
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
-                      <a:srgbClr val="000000"/>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" b="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:rPr>
+                  <a:rPr lang="en-US"/>
                   <a:t>Gross Output</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
           <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln/>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
-            <a:pPr lvl="0">
-              <a:defRPr b="0">
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:srgbClr val="000000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -1153,17 +1542,1132 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
     <c:showDLblsOverMax val="1"/>
   </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1651,7 +3155,9 @@
   </sheetPr>
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
@@ -1895,8 +3401,8 @@
   </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>